<commit_message>
Currently creates a full S9000 config
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wblankenship\Documents\NIA Work Documents\FE\ASE SPT Protocol Translator Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wblankenship\Documents\GitHub\SPT-Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CC72F1-377E-4097-8C3F-FEAD1791EAD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65CBD74-D4E8-48E8-B99A-A2E043B51EC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D2F1E244-0055-49E9-BA99-E37AFD162BFC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="49">
   <si>
     <t>BK 1 VCB</t>
   </si>
@@ -87,12 +87,6 @@
     <t>DX RELAY FAIL</t>
   </si>
   <si>
-    <t xml:space="preserve">LOSS OF POTENTIAL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BK 1 CKT INT CI-2/SEL TRBL  </t>
-  </si>
-  <si>
     <t>ADAPTIVE RELAYING</t>
   </si>
   <si>
@@ -180,7 +174,10 @@
     <t xml:space="preserve">c31 was undefined but I deleted it for the program to create the correct number of control points. Need to put in an if statement to not create a point if the point is undefined or undef. . Etc. . . </t>
   </si>
   <si>
-    <t>None</t>
+    <t>BK 1 CKT INT CI-2/SEL TRBL</t>
+  </si>
+  <si>
+    <t>LOSS OF POTENTIAL</t>
   </si>
 </sst>
 </file>
@@ -539,7 +536,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,6 +544,7 @@
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -554,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
@@ -566,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -574,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -586,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -594,19 +592,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -614,19 +612,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -634,19 +632,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -654,19 +652,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -674,19 +672,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -694,19 +692,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -714,19 +712,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -734,19 +732,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -754,19 +752,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -774,19 +772,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,13 +792,13 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -808,13 +806,13 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -822,13 +820,13 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -836,13 +834,13 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -850,13 +848,13 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -864,13 +862,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -878,13 +876,13 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -892,13 +890,13 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -906,13 +904,13 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -920,13 +918,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -934,13 +932,13 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -948,183 +946,177 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F31" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>48</v>
+        <v>20</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="H34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="H35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>